<commit_message>
REPORTGEN-870: update chinese library reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/zh-CN/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/zh-CN/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19D6B41-8536-4474-9A23-AA67A7DFEAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D0333D-AFA8-4538-82D0-F07F0EBCDFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="-12840" windowWidth="21600" windowHeight="11325" tabRatio="701" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11325" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="274">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -583,9 +583,6 @@
   </si>
   <si>
     <t>* Block Name = RULES_LIST_STATISTICS_RATIO</t>
-  </si>
-  <si>
-    <t>* METRICS=List of metrics id (BC, TC or QR) or quality standards tags separated by ‘|’.</t>
   </si>
   <si>
     <t>* CRITICAL=true : add this option if you have selected a BC or a TC and want only critical rules to be selected (by default it is false). This option has no effect on selection by QR or quality standard tag.</t>
@@ -947,9 +944,6 @@
     <t>* Block Name = QUALITY_TAGS_RULES_EVOLUTION</t>
   </si>
   <si>
-    <t>* STD= Name of the quality standard category for which you want the details per tag, for example, STIG-V4R8-CAT1 will list total, added and removed violations for cast rules associated to all tags belonged to category STIG-V4R8-CAT1</t>
-  </si>
-  <si>
     <t>To use this component, the Quality Standards Mapping extension should be installed on the central where the application resides, with minimum version 20190624</t>
   </si>
   <si>
@@ -1053,6 +1047,18 @@
   </si>
   <si>
     <t>RepGen:TEXT;METRIC_EVOLUTION;ID=60017</t>
+  </si>
+  <si>
+    <t>* METRICS=List of metrics id (BC, TC or QR) or quality standards tags separated by ‘|’. It can also be the name for a BC or a shortName for a TC</t>
+  </si>
+  <si>
+    <t>UPDATED</t>
+  </si>
+  <si>
+    <t>* STD= Name of the quality standard category, or BC name, or BC id, for which you want the details per tag or TC, for example, STIG-V4R8-CAT1 will list total, added and removed violations for cast rules associated to all tags belonged to category STIG-V4R8-CAT1</t>
+  </si>
+  <si>
+    <t>The STD parameter can also take the name, shortName or ID os a Business Criterion</t>
   </si>
 </sst>
 </file>
@@ -1771,33 +1777,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
     </row>
-    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1805,7 +1811,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="3"/>
@@ -1813,7 +1819,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="3"/>
@@ -1821,54 +1827,54 @@
       <c r="F4" s="1"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="17"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="10" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
         <v>77</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="13" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
@@ -1876,7 +1882,7 @@
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
@@ -1884,7 +1890,7 @@
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
       <c r="F23" s="11"/>
     </row>
@@ -1907,75 +1913,82 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
-  <dimension ref="B1:C13"/>
+  <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23"/>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="22"/>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1992,103 +2005,103 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="30" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="30" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>247</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="30" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="30" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2105,53 +2118,53 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="22"/>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2168,52 +2181,52 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="26"/>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="I1" s="26"/>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
     </row>
   </sheetData>
@@ -2230,88 +2243,88 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="25" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B12" s="25" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="25" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="25" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B15" s="25" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2328,56 +2341,56 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
     </row>
   </sheetData>
@@ -2394,46 +2407,46 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23"/>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
     </row>
   </sheetData>
@@ -2450,64 +2463,66 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23"/>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="22"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2524,53 +2539,53 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
-    <col min="3" max="3" width="109.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="23"/>
-    </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23"/>
-    </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2583,77 +2598,77 @@
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
-    <col min="3" max="3" width="109.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="28" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="28" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2666,709 +2681,709 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="18" customWidth="1"/>
     <col min="6" max="7" width="38" style="18" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.109375" style="18"/>
-    <col min="11" max="11" width="14.33203125" style="18" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" style="18" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="18"/>
+    <col min="8" max="8" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="18"/>
+    <col min="11" max="11" width="14.28515625" style="18" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="18" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B53" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B58" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B63" s="19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B73" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B78" s="19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B83" s="19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B88" s="19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="95" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B95" s="19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="102" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B102" s="19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="109" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B109" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B114" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B119" s="19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B124" s="19" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B129" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B134" s="19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B143" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B144" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B145" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B146" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B147" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B148" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B149" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="18" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="152" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B152" s="19" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" s="18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154" s="18" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B153" s="18" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B154" s="18" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" s="21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158" s="21" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159" s="21" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160" s="18" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B157" s="21" t="s">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B161" s="18" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B158" s="21" t="s">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162" s="18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163" s="18" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B159" s="21" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B160" s="18" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B161" s="18" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B162" s="18" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B163" s="18" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3385,19 +3400,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -3405,7 +3420,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -3413,7 +3428,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>72</v>
       </c>
@@ -3421,7 +3436,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -3439,32 +3454,32 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>60</v>
       </c>
@@ -3472,7 +3487,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>62</v>
       </c>
@@ -3480,7 +3495,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>64</v>
       </c>
@@ -3488,19 +3503,19 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3523,22 +3538,22 @@
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>82</v>
       </c>
@@ -3546,7 +3561,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>83</v>
       </c>
@@ -3554,7 +3569,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>84</v>
       </c>
@@ -3562,7 +3577,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>85</v>
       </c>
@@ -3570,7 +3585,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>86</v>
       </c>
@@ -3578,7 +3593,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>87</v>
       </c>
@@ -3586,7 +3601,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>88</v>
       </c>
@@ -3594,7 +3609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>89</v>
       </c>
@@ -3602,7 +3617,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>90</v>
       </c>
@@ -3610,7 +3625,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>102</v>
       </c>
@@ -3618,8 +3633,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>101</v>
       </c>
@@ -3637,92 +3652,92 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>146</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>147</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>164</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>150</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>148</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -3741,47 +3756,47 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>171</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>153</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>154</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>155</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -20167,35 +20182,35 @@
       <c r="XFC6" s="22"/>
       <c r="XFD6" s="22"/>
     </row>
-    <row r="7" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>156</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -20214,62 +20229,62 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>160</v>
       </c>
@@ -20287,90 +20302,92 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="29" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="24"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="C7" s="24"/>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>251</v>
-      </c>
-      <c r="C9" s="24"/>
-    </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="24"/>
-    </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-1021: update chinese reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/zh-CN/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/zh-CN/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AA0B77-9C39-41EF-A8DA-FCB73FB77437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A11332-B277-46F6-9C82-D8E513DEB76A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="2505" windowWidth="21075" windowHeight="11385" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="287">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -881,9 +881,6 @@
     <t>* Block Name = AETP_LIST</t>
   </si>
   <si>
-    <t>RepGen:TABLE;AETP_LIST;COUNT=-1</t>
-  </si>
-  <si>
     <r>
       <t>CRITICITY =</t>
     </r>
@@ -1097,6 +1094,12 @@
   </si>
   <si>
     <t>* TAG=YES|NO, to display the priority using tag or priority (tag by default as this is this value that is set in ED)</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;AETP_LIST;COUNT=-1,FORMAT=N2</t>
+  </si>
+  <si>
+    <t>FORMAT: The number of decimals for effort complexity, ratio and AETP count (N2 for 2 decimals, N5 for 5 decimals), by default N2.</t>
   </si>
 </sst>
 </file>
@@ -1815,7 +1818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1964,7 +1967,7 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C1" s="29"/>
     </row>
@@ -1980,27 +1983,27 @@
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2084,22 +2087,22 @@
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2127,7 +2130,7 @@
     </row>
     <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -2137,7 +2140,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -2251,7 +2254,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2259,7 +2262,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2415,7 +2418,7 @@
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
@@ -2442,10 +2445,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822C81FE-2BA1-4A3C-ADB8-F42B4B1305BA}">
-  <dimension ref="B1:B8"/>
+  <dimension ref="B1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2474,21 +2477,26 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2511,33 +2519,33 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2550,7 +2558,7 @@
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2561,7 +2569,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2586,18 +2594,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2613,7 +2621,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2624,7 +2632,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2648,18 +2656,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2669,12 +2677,12 @@
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2692,12 +2700,12 @@
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2707,7 +2715,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3027,17 +3035,17 @@
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
@@ -3047,27 +3055,27 @@
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="81" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -3337,7 +3345,7 @@
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
@@ -3347,12 +3355,12 @@
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
@@ -3402,7 +3410,7 @@
     </row>
     <row r="158" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B158" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
@@ -3412,17 +3420,17 @@
     </row>
     <row r="161" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B161" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
@@ -3432,27 +3440,27 @@
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
@@ -3462,37 +3470,37 @@
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -3513,32 +3521,32 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3556,12 +3564,12 @@
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3698,18 +3706,18 @@
     </row>
     <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>276</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="7" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>278</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3961,7 +3969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F8858A-750A-4726-A1F9-D59D03327DAC}">
   <dimension ref="B1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4007,7 +4015,7 @@
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -4151,7 +4159,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4171,25 +4179,25 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C7" s="24"/>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C8" s="24"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C9" s="24"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C10" s="24"/>
     </row>

</xml_diff>

<commit_message>
REPORTGEN-1082: update chinese library components
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/zh-CN/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/zh-CN/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7620B41-E86B-42FD-99CC-F4C127C3DC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5756E228-475F-40A0-BFAF-DADB04FAFF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="846" firstSheet="14" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="3-OMGTechDebt" sheetId="30" r:id="rId21"/>
     <sheet name="3-OMGTechDebtDetails" sheetId="31" r:id="rId22"/>
     <sheet name="3 - Evolution of iso TD" sheetId="32" r:id="rId23"/>
+    <sheet name="3 - Rules evolution reg. Omg TD" sheetId="33" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="317">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1274,6 +1275,44 @@
   </si>
   <si>
     <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_EVOLUTION;ID=ISO,MORE=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>* Block Name = OMG_TECHNICAL_DEBT_EVOLUTION</t>
+  </si>
+  <si>
+    <t>* Block Name = OMG_TECHNICAL_DEBT_RULES_EVOLUTION</t>
+  </si>
+  <si>
+    <r>
+      <t>- ID=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>name of index, like ‘ISO-5055-Security’</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>DESC=true : add this one if you want to display the rules descriptions (false by default)</t>
+    </r>
+  </si>
+  <si>
+    <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_RULES_EVOLUTION;ID=ISO-5055-Security,DESC=true,HEADER=NO</t>
   </si>
 </sst>
 </file>
@@ -1545,7 +1584,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1613,6 +1652,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1628,7 +1670,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2012,7 +2054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -2035,8 +2077,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -2047,16 +2089,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -2104,26 +2146,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -3974,7 +4016,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F19727-0A4D-46F0-B892-29E8A396F1FB}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C80DEE1-1402-4F3F-9664-8981C357215E}">
+  <dimension ref="B1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3991,55 +4111,50 @@
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>176</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
-        <v>309</v>
+      <c r="B3" s="33" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
-        <v>306</v>
+      <c r="B4" s="39" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>290</v>
-      </c>
+      <c r="B10" s="25"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="25"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>311</v>
+      <c r="B11" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>